<commit_message>
Creating rows for each row in PDF
</commit_message>
<xml_diff>
--- a/updated_pdfs/test_file.xlsx
+++ b/updated_pdfs/test_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="17">
   <si>
     <t>Job NumberRow1</t>
   </si>
@@ -31,97 +31,40 @@
     <t>Total OT Hrs</t>
   </si>
   <si>
-    <t>Regularhrs1</t>
-  </si>
-  <si>
-    <t>Regularhrs2</t>
-  </si>
-  <si>
-    <t>Regularhrs3</t>
-  </si>
-  <si>
-    <t>Regularhrs4</t>
-  </si>
-  <si>
-    <t>Regularhrs5</t>
-  </si>
-  <si>
-    <t>Regularhrs6</t>
-  </si>
-  <si>
-    <t>Regularhrs7</t>
-  </si>
-  <si>
-    <t>Overtimehrs1</t>
-  </si>
-  <si>
-    <t>Overtimehrs2</t>
-  </si>
-  <si>
-    <t>Overtimehrs3</t>
-  </si>
-  <si>
-    <t>Overtimehrs4</t>
-  </si>
-  <si>
-    <t>Overtimehrs5</t>
-  </si>
-  <si>
-    <t>Overtimehrs6</t>
-  </si>
-  <si>
-    <t>Overtimehrs7</t>
-  </si>
-  <si>
-    <t>Super1</t>
-  </si>
-  <si>
-    <t>Super2</t>
-  </si>
-  <si>
-    <t>Super3</t>
-  </si>
-  <si>
-    <t>Super4</t>
-  </si>
-  <si>
-    <t>Super5</t>
-  </si>
-  <si>
-    <t>Super6</t>
-  </si>
-  <si>
-    <t>Super7</t>
+    <t>Regularhrs</t>
+  </si>
+  <si>
+    <t>Overtimehrs</t>
+  </si>
+  <si>
+    <t>Super</t>
   </si>
   <si>
     <t>107</t>
   </si>
   <si>
-    <t>Bob Bailey</t>
-  </si>
-  <si>
-    <t>27263</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>Billy Porterfield</t>
+  </si>
+  <si>
+    <t>990</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3107</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>18698</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18698 </t>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -479,41 +422,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
-    <col min="26" max="26" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,124 +463,160 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>990</v>
+      </c>
+      <c r="D2">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C3">
+        <v>990</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>990</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>990</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>990</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>990</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="E8" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added earn code functionailty
</commit_message>
<xml_diff>
--- a/updated_pdfs/test_file.xlsx
+++ b/updated_pdfs/test_file.xlsx
@@ -14,21 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="17">
-  <si>
-    <t>Job NumberRow1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="26">
+  <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Today Date</t>
+  </si>
+  <si>
+    <t>jcco</t>
+  </si>
+  <si>
+    <t>Job NumberRow</t>
+  </si>
+  <si>
+    <t>CostPhase CodeRow</t>
   </si>
   <si>
     <t>Employee Name</t>
   </si>
   <si>
-    <t>Employee Number</t>
-  </si>
-  <si>
-    <t>Total Hrs</t>
-  </si>
-  <si>
-    <t>Total OT Hrs</t>
+    <t xml:space="preserve">Class Line </t>
   </si>
   <si>
     <t>Regularhrs</t>
@@ -37,34 +43,55 @@
     <t>Overtimehrs</t>
   </si>
   <si>
+    <t xml:space="preserve">Equip Repaired </t>
+  </si>
+  <si>
     <t>Super</t>
   </si>
   <si>
+    <t>earn</t>
+  </si>
+  <si>
+    <t>27263</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>107</t>
   </si>
   <si>
-    <t>Billy Porterfield</t>
-  </si>
-  <si>
-    <t>990</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>Bob Bailey</t>
+  </si>
+  <si>
+    <t>0501</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>91979</t>
+  </si>
+  <si>
     <t>3107</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>1</t>
+    <t>960013</t>
+  </si>
+  <si>
+    <t>52206</t>
+  </si>
+  <si>
+    <t>6080</t>
+  </si>
+  <si>
+    <t>802-PTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -422,23 +449,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,160 +494,196 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
+        <v>27263</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>107</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>990</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>501</v>
+      </c>
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="J2">
+        <v>91979</v>
+      </c>
+      <c r="K2">
         <v>3107</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
+        <v>27263</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>990</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>501</v>
+      </c>
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>960013</v>
+      </c>
+      <c r="K3">
         <v>3107</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
+        <v>27263</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>107</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>990</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>15</v>
       </c>
       <c r="G4">
+        <v>501</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
         <v>3107</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
+        <v>27263</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>107</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>990</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
       <c r="E5">
-        <v>5</v>
+        <v>6080</v>
       </c>
       <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5">
         <v>3107</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
-        <v>107</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
+        <v>27263</v>
       </c>
       <c r="C6">
-        <v>990</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>3107</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>27263</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>990</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>